<commit_message>
Final updates for VA creation
</commit_message>
<xml_diff>
--- a/Alaska VADAM Ties.xlsx
+++ b/Alaska VADAM Ties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,17 +442,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>800577</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>801740</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>803260</v>
+        <v>800021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added end agreement functions
</commit_message>
<xml_diff>
--- a/Alaska VADAM Ties.xlsx
+++ b/Alaska VADAM Ties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,42 +442,37 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3350</v>
+        <v>672501</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>433788</v>
+        <v>724629</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>641752</v>
+        <v>800318</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>800523</v>
+        <v>801131</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>801170</v>
+        <v>801254</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>802154</v>
+        <v>801557</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>805430</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>806538</v>
+        <v>806186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added va end process and ca create process, but not ca end nor va/ca void process
</commit_message>
<xml_diff>
--- a/Alaska VADAM Ties.xlsx
+++ b/Alaska VADAM Ties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,37 +442,12 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>672501</v>
+        <v>801330</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>724629</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>800318</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>801131</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>801254</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>801557</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>806186</v>
+        <v>801835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
up to date goodies
</commit_message>
<xml_diff>
--- a/Alaska VADAM Ties.xlsx
+++ b/Alaska VADAM Ties.xlsx
@@ -442,12 +442,12 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>801330</v>
+        <v>701775</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>801835</v>
+        <v>802332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to format and integrating digital deals
</commit_message>
<xml_diff>
--- a/Alaska VADAM Ties.xlsx
+++ b/Alaska VADAM Ties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,12 +442,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>701775</v>
+        <v>344836</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>802332</v>
+        <v>641515</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>684562</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>800266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>